<commit_message>
Update to graphs and re-configurement of main
schedMain should be set up to run as an individual program to run one procList
</commit_message>
<xml_diff>
--- a/ProcessSimulator/ExternalPriorityTests.xlsx
+++ b/ProcessSimulator/ExternalPriorityTests.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jared Allen\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Documents\MST\Fall 2020\CS 3800\Project\Simulator\Process-Memory-Mangaement-Simulation\ProcessSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8E4E61-3284-4CD5-AAEE-3EB98E14AB27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C41409-33C4-4F6B-A5BE-8C596C0E5C58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="23">
   <si>
     <t>Input</t>
   </si>
@@ -81,6 +81,27 @@
   </si>
   <si>
     <t>RR quantum = 4</t>
+  </si>
+  <si>
+    <t>Response Ratio Quantum</t>
+  </si>
+  <si>
+    <t>Khigh Quantum</t>
+  </si>
+  <si>
+    <t>Low Quantum</t>
+  </si>
+  <si>
+    <t>Ep Multiplier</t>
+  </si>
+  <si>
+    <t>Modified HRRN Runtime</t>
+  </si>
+  <si>
+    <t>Multilevel Queue Runtime</t>
+  </si>
+  <si>
+    <t>Multilevel Feedback Queue Runtime</t>
   </si>
 </sst>
 </file>
@@ -3056,16 +3077,13 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr>
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:sysClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -6496,10 +6514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS109"/>
+  <dimension ref="A1:AS121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T163" sqref="T163"/>
+    <sheetView tabSelected="1" topLeftCell="P94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AG114" sqref="AG114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17921,8 +17939,101 @@
         <v>8</v>
       </c>
     </row>
+    <row r="118" spans="29:35" x14ac:dyDescent="0.25">
+      <c r="AC118" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD118" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE118" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF118" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG118" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH118" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI118" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="119" spans="29:35" x14ac:dyDescent="0.25">
+      <c r="AC119">
+        <v>2</v>
+      </c>
+      <c r="AD119">
+        <v>5</v>
+      </c>
+      <c r="AE119">
+        <v>7</v>
+      </c>
+      <c r="AF119">
+        <v>0.5</v>
+      </c>
+      <c r="AG119">
+        <v>3944192.1782178218</v>
+      </c>
+      <c r="AH119">
+        <v>1178999.207920792</v>
+      </c>
+      <c r="AI119">
+        <v>1229387.712871287</v>
+      </c>
+    </row>
+    <row r="120" spans="29:35" x14ac:dyDescent="0.25">
+      <c r="AC120">
+        <v>2</v>
+      </c>
+      <c r="AD120">
+        <v>3</v>
+      </c>
+      <c r="AE120">
+        <v>4</v>
+      </c>
+      <c r="AF120">
+        <v>1</v>
+      </c>
+      <c r="AG120">
+        <v>3906055.9801980196</v>
+      </c>
+      <c r="AH120">
+        <v>1188446.1485148515</v>
+      </c>
+      <c r="AI120">
+        <v>1172793.2772277228</v>
+      </c>
+    </row>
+    <row r="121" spans="29:35" x14ac:dyDescent="0.25">
+      <c r="AC121">
+        <v>4</v>
+      </c>
+      <c r="AD121">
+        <v>7</v>
+      </c>
+      <c r="AE121">
+        <v>13</v>
+      </c>
+      <c r="AF121">
+        <v>2</v>
+      </c>
+      <c r="AG121">
+        <v>4009024.207920792</v>
+      </c>
+      <c r="AH121">
+        <v>1185012.207920792</v>
+      </c>
+      <c r="AI121">
+        <v>1191264.5841584159</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>